<commit_message>
feat: Updated CAD models
Poses shown in all examples. Also fixed some reference to linked .xls files.
</commit_message>
<xml_diff>
--- a/Example- Demo/5US Platform/Components/Coupler param.xlsx
+++ b/Example- Demo/5US Platform/Components/Coupler param.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshel\Documents\GitHub\5ss-platform-synthesis\Example- Demo\5US Platform\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011FCB63-9D60-4122-8488-94A1430E03F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76002D35-1499-4A9C-A522-38289CAFF282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J2" sqref="J2:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -419,131 +419,131 @@
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <f>J2</f>
-        <v>1.24563</v>
+        <v>-3.6908300000000001</v>
       </c>
       <c r="B2" s="2">
         <f>K2</f>
-        <v>-11.8165</v>
+        <v>3.6051000000000002</v>
       </c>
       <c r="C2" s="2">
         <f>L2</f>
-        <v>0.20905099999999999</v>
+        <v>0.72284099999999996</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J2">
-        <v>1.24563</v>
+        <v>-3.6908300000000001</v>
       </c>
       <c r="K2">
-        <v>-11.8165</v>
+        <v>3.6051000000000002</v>
       </c>
       <c r="L2">
-        <v>0.20905099999999999</v>
+        <v>0.72284099999999996</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A6" si="0">J3</f>
-        <v>1.9200900000000001</v>
+        <v>4.8814500000000001</v>
       </c>
       <c r="B3" s="2">
         <f t="shared" ref="B3:B6" si="1">K3</f>
-        <v>-0.725383</v>
+        <v>-1.55169</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C6" si="2">L3</f>
-        <v>-0.18651799999999999</v>
+        <v>-5.5954300000000003</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J3">
-        <v>1.9200900000000001</v>
+        <v>4.8814500000000001</v>
       </c>
       <c r="K3">
-        <v>-0.725383</v>
+        <v>-1.55169</v>
       </c>
       <c r="L3">
-        <v>-0.18651799999999999</v>
+        <v>-5.5954300000000003</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
-        <v>-2.28999</v>
+        <v>-7.3979299999999997</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" si="1"/>
-        <v>-9.6036000000000001</v>
+        <v>0.53811799999999999</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="2"/>
-        <v>-2.46123E-2</v>
+        <v>7.1681400000000002</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J4">
-        <v>-2.28999</v>
+        <v>-7.3979299999999997</v>
       </c>
       <c r="K4">
-        <v>-9.6036000000000001</v>
+        <v>0.53811799999999999</v>
       </c>
       <c r="L4">
-        <v>-2.46123E-2</v>
+        <v>7.1681400000000002</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
-        <v>13.082800000000001</v>
+        <v>0.68991400000000003</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" si="1"/>
-        <v>-2.4093800000000001</v>
+        <v>-4.21556</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="2"/>
-        <v>-1.5715699999999999</v>
+        <v>1.69537</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J5">
-        <v>13.082800000000001</v>
+        <v>0.68991400000000003</v>
       </c>
       <c r="K5">
-        <v>-2.4093800000000001</v>
+        <v>-4.21556</v>
       </c>
       <c r="L5">
-        <v>-1.5715699999999999</v>
+        <v>1.69537</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
-        <v>22.874700000000001</v>
+        <v>-2.8578199999999998</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" si="1"/>
-        <v>-1.5944700000000001</v>
+        <v>-16.145800000000001</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="2"/>
-        <v>-5.2618</v>
+        <v>14.116300000000001</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J6">
-        <v>22.874700000000001</v>
+        <v>-2.8578199999999998</v>
       </c>
       <c r="K6">
-        <v>-1.5944700000000001</v>
+        <v>-16.145800000000001</v>
       </c>
       <c r="L6">
-        <v>-5.2618</v>
+        <v>14.116300000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>